<commit_message>
more work on report, conclusion to do
</commit_message>
<xml_diff>
--- a/TravellingSalesman/TravellingSalesman/Solutions/Collated Results.xlsx
+++ b/TravellingSalesman/TravellingSalesman/Solutions/Collated Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="890" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="890"/>
   </bookViews>
   <sheets>
     <sheet name="Totals" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="9">
   <si>
     <t>Two-Opt Time (ms)</t>
   </si>
@@ -37,27 +37,35 @@
     <t>NN Length</t>
   </si>
   <si>
-    <t>DataSet</t>
-  </si>
-  <si>
     <t>Dimension</t>
   </si>
   <si>
-    <t>NN Time</t>
+    <t>Nearest Neighbour</t>
   </si>
   <si>
-    <t>2-Opt Length</t>
+    <t>Two-Opt</t>
   </si>
   <si>
-    <t>2-Opt Time</t>
+    <t>Time (ms)</t>
+  </si>
+  <si>
+    <t>Length (units)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -73,7 +81,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -81,13 +89,274 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -120,6 +389,35 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Two</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t>-Opt Time Vs Dimension</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -157,14 +455,14 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.10470860874832118"/>
-          <c:y val="8.3198743831314495E-2"/>
-          <c:w val="0.78915984164186836"/>
-          <c:h val="0.86634697244271119"/>
+          <c:x val="0.16196821996941266"/>
+          <c:y val="0.13506548202655666"/>
+          <c:w val="0.79522462817147854"/>
+          <c:h val="0.72088764946048411"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -195,7 +493,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Totals!$B$3:$B$11</c:f>
+              <c:f>Totals!$C$4:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -231,108 +529,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Totals!$D$3:$D$11</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>11.6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>18.399999999999999</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44.6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Totals!$B$3:$B$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>52</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>159</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>318</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>574</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>783</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1002</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1432</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Totals!$F$3:$F$11</c:f>
+              <c:f>Totals!$G$4:$G$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="9"/>
@@ -366,7 +563,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -376,11 +573,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="450037096"/>
-        <c:axId val="450046504"/>
+        <c:axId val="252781704"/>
+        <c:axId val="254392784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="450037096"/>
+        <c:axId val="252781704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -400,6 +597,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Dimension</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> (Problem Size)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -437,12 +695,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="450046504"/>
+        <c:crossAx val="254392784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="450046504"/>
+        <c:axId val="254392784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -462,7 +720,68 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Taken to Complete Algorithm (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -499,9 +818,604 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="450037096"/>
+        <c:crossAx val="252781704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Comparison</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> of Algorithms Against Time</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Nearest Neighbour</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Totals!$C$4:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>318</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>574</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>783</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1432</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Totals!$E$4:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Two-Opt</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Totals!$C$4:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>318</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>574</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>783</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1432</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Totals!$G$4:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>831.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2204.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6512.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12134.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44130</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>119372.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>260423.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>662562.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="254388080"/>
+        <c:axId val="254391216"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="254388080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Dimension</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> (Problem Size)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="254391216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="254391216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="700000"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time to</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Complete Algorithm (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="254388080"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="100000"/>
+        <c:minorUnit val="20000"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -580,7 +1494,579 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t>Nearest Neighbour Time Vs Dimension</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13471506739623648"/>
+          <c:y val="0.13921212490191304"/>
+          <c:w val="0.79522462817147854"/>
+          <c:h val="0.72088764946048411"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Nearest</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Totals!$C$4:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>318</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>574</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>783</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1432</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Totals!$E$4:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="254388864"/>
+        <c:axId val="254390040"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="254388864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Dimension</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> (Problem Size)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="254390040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="254390040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Taken to Complete Algorithm (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="254388864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1136,24 +2622,1056 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>586740</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>464820</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>106680</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1163,6 +3681,68 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>541020</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>148590</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>586740</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1458,257 +4038,298 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F11"/>
+  <dimension ref="B1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="21"/>
+      <c r="F2" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="21"/>
+    </row>
+    <row r="3" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="13"/>
+      <c r="C3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F3" s="10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
+      <c r="G3" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B4" s="2"/>
+      <c r="C4" s="16">
         <v>52</v>
       </c>
-      <c r="C3">
+      <c r="D4" s="18">
         <f>AVERAGE('DataSet-berlin52'!A2:A6)</f>
         <v>8980.9182793291893</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E4" s="19">
         <f>AVERAGE('DataSet-u159'!B2:B6)</f>
         <v>0</v>
       </c>
-      <c r="E3">
+      <c r="F4" s="7">
         <f>AVERAGE('DataSet-berlin52'!C2:C6)</f>
         <v>8114.3541033990796</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G4" s="8">
         <f>AVERAGE('DataSet-berlin52'!D2:D6)</f>
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
+      <c r="I4">
+        <f>D4/F4</f>
+        <v>1.1067939807516052</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B5" s="2"/>
+      <c r="C5" s="16">
         <v>159</v>
       </c>
-      <c r="C4">
+      <c r="D5" s="5">
         <f>AVERAGE('DataSet-u159'!A2:A6)</f>
         <v>54669.026414963402</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E5" s="3">
         <f>AVERAGE('DataSet-u159'!B2:B6)</f>
         <v>0</v>
       </c>
-      <c r="E4">
+      <c r="F5" s="5">
         <f>AVERAGE('DataSet-u159'!C2:C6)</f>
         <v>46254.183212226199</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G5" s="3">
         <f>AVERAGE('DataSet-u159'!D2:D6)</f>
         <v>831.2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5">
+      <c r="I5">
+        <f t="shared" ref="I5:I12" si="0">D5/F5</f>
+        <v>1.1819261009134616</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B6" s="2"/>
+      <c r="C6" s="16">
         <v>200</v>
       </c>
-      <c r="C5">
+      <c r="D6" s="5">
         <f>AVERAGE('DataSet-kroA200'!A2:A6)</f>
         <v>35798.408974281898</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E6" s="3">
         <f>AVERAGE('DataSet-kroA200'!B2:B6)</f>
         <v>0.4</v>
       </c>
-      <c r="E5">
+      <c r="F6" s="5">
         <f>AVERAGE('DataSet-kroA200'!C2:C6)</f>
         <v>30514.964491648501</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G6" s="3">
         <f>AVERAGE('DataSet-kroA200'!D2:D6)</f>
         <v>2204.4</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6">
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>1.1731427373634795</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B7" s="2"/>
+      <c r="C7" s="16">
         <v>318</v>
       </c>
-      <c r="C6">
+      <c r="D7" s="5">
         <f>AVERAGE('DataSet-lin318'!A2:A6)</f>
         <v>54033.576773283399</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E7" s="3">
         <f>AVERAGE('DataSet-lin318'!B2:B6)</f>
         <v>1.4</v>
       </c>
-      <c r="E6">
+      <c r="F7" s="5">
         <f>AVERAGE('DataSet-lin318'!C2:C6)</f>
         <v>45464.807390407099</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G7" s="3">
         <f>AVERAGE('DataSet-lin318'!D2:D6)</f>
         <v>6512.6</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7">
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>1.1884703768630565</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B8" s="2"/>
+      <c r="C8" s="16">
         <v>400</v>
       </c>
-      <c r="C7">
+      <c r="D8" s="5">
         <f>AVERAGE('DataSet-rd400'!A2:A6)</f>
         <v>19168.0516099099</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E8" s="3">
         <f>AVERAGE('DataSet-rd400'!B2:B6)</f>
         <v>3</v>
       </c>
-      <c r="E7">
+      <c r="F8" s="5">
         <f>AVERAGE('DataSet-rd400'!C2:C6)</f>
         <v>16393.570077607099</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G8" s="3">
         <f>AVERAGE('DataSet-rd400'!D2:D6)</f>
         <v>12134.8</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8">
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>1.1692420576584854</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="2"/>
+      <c r="C9" s="16">
         <v>574</v>
       </c>
-      <c r="C8">
+      <c r="D9" s="5">
         <f>AVERAGE('DataSet-u574'!A2:A6)</f>
         <v>46881.8660383116</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E9" s="3">
         <f>AVERAGE('DataSet-u574'!B2:B6)</f>
         <v>6</v>
       </c>
-      <c r="E8">
+      <c r="F9" s="5">
         <f>AVERAGE('DataSet-u574'!C2:C6)</f>
         <v>40031.736801804</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G9" s="3">
         <f>AVERAGE('DataSet-u574'!D2:D6)</f>
         <v>44130</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9">
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>1.1711174628875685</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="2"/>
+      <c r="C10" s="16">
         <v>783</v>
       </c>
-      <c r="C9">
+      <c r="D10" s="5">
         <f>AVERAGE('DataSet-rat783'!A2:A6)</f>
         <v>11255.0702449622</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E10" s="3">
         <f>AVERAGE('DataSet-rat783'!B2:B6)</f>
         <v>11.6</v>
       </c>
-      <c r="E9">
+      <c r="F10" s="5">
         <f>AVERAGE('DataSet-rat783'!C2:C6)</f>
         <v>9619.3289596669401</v>
       </c>
-      <c r="F9" s="1">
+      <c r="G10" s="3">
         <f>AVERAGE('DataSet-rat783'!D2:D6)</f>
         <v>119372.6</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10">
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>1.1700473382450887</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="2"/>
+      <c r="C11" s="16">
         <v>1002</v>
       </c>
-      <c r="C10">
+      <c r="D11" s="5">
         <f>AVERAGE('DataSet-pr1002'!A2:A6)</f>
         <v>315596.58739424299</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E11" s="3">
         <f>AVERAGE('DataSet-pr1002'!B2:B6)</f>
         <v>18.399999999999999</v>
       </c>
-      <c r="E10">
+      <c r="F11" s="5">
         <f>AVERAGE('DataSet-pr1002'!C2:C6)</f>
         <v>276051.47264864302</v>
       </c>
-      <c r="F10" s="1">
+      <c r="G11" s="3">
         <f>AVERAGE('DataSet-pr1002'!D2:D6)</f>
         <v>260423.6</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11">
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>1.1432526853277569</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="2"/>
+      <c r="C12" s="17">
         <v>1432</v>
       </c>
-      <c r="C11">
+      <c r="D12" s="6">
         <f>AVERAGE('DataSet-u1432'!A2:A6)</f>
         <v>188815.01032068199</v>
       </c>
-      <c r="D11" s="1">
+      <c r="E12" s="4">
         <f>AVERAGE('DataSet-u1432'!B2:B6)</f>
         <v>44.6</v>
       </c>
-      <c r="E11">
+      <c r="F12" s="6">
         <f>AVERAGE('DataSet-u1432'!C2:C6)</f>
         <v>166349.170336657</v>
       </c>
-      <c r="F11" s="1">
+      <c r="G12" s="4">
         <f>AVERAGE('DataSet-u1432'!D2:D6)</f>
         <v>662562.4</v>
       </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>1.1350523115838731</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I13">
+        <f>AVERAGE(I4:I12)</f>
+        <v>1.1598938946215975</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -2517,8 +5138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>